<commit_message>
Rename console->sys_out, since console does other stuff actually
</commit_message>
<xml_diff>
--- a/LLVMFunctionTracking.xlsx
+++ b/LLVMFunctionTracking.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="86" documentId="8_{D9D57C98-AA63-462C-A3D4-1915862581C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9641A593-8029-46E4-8FAE-299098F4F6EC}"/>
+  <xr:revisionPtr revIDLastSave="109" documentId="8_{D9D57C98-AA63-462C-A3D4-1915862581C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F85242DD-36E5-457D-8BD1-C12EACE413BF}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BE9E4DA6-7603-4761-9EA2-AD44CBE23B5C}"/>
   </bookViews>
@@ -1376,14 +1376,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Output" xfId="2" builtinId="21"/>
   </cellStyles>
-  <dxfs count="8">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <fill>
         <patternFill>
@@ -1394,35 +1387,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1745,8 +1710,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{256DFC43-7668-41A4-8C27-D4E103314C5D}">
   <dimension ref="A1:I363"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A220" workbookViewId="0">
-      <selection activeCell="C248" sqref="C248"/>
+    <sheetView tabSelected="1" topLeftCell="A291" workbookViewId="0">
+      <selection activeCell="C318" sqref="C318"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2620,7 +2585,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" s="4" t="s">
         <v>95</v>
       </c>
@@ -2628,7 +2593,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" s="4" t="s">
         <v>96</v>
       </c>
@@ -2636,7 +2601,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" s="4" t="s">
         <v>97</v>
       </c>
@@ -2644,7 +2609,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" s="4" t="s">
         <v>98</v>
       </c>
@@ -2652,7 +2617,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" s="4" t="s">
         <v>99</v>
       </c>
@@ -2660,7 +2625,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" s="4" t="s">
         <v>100</v>
       </c>
@@ -2668,7 +2633,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" s="4" t="s">
         <v>101</v>
       </c>
@@ -2676,7 +2641,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" s="4" t="s">
         <v>102</v>
       </c>
@@ -2684,7 +2649,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" s="4" t="s">
         <v>103</v>
       </c>
@@ -2692,7 +2657,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" s="4" t="s">
         <v>104</v>
       </c>
@@ -2700,7 +2665,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" s="4" t="s">
         <v>105</v>
       </c>
@@ -2708,7 +2673,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" s="4" t="s">
         <v>106</v>
       </c>
@@ -2716,7 +2681,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" s="4" t="s">
         <v>107</v>
       </c>
@@ -2724,7 +2689,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" s="4" t="s">
         <v>108</v>
       </c>
@@ -2732,18 +2697,15 @@
         <v>364</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" s="4" t="s">
         <v>109</v>
       </c>
       <c r="B111" t="s">
-        <v>366</v>
-      </c>
-      <c r="C111" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" s="4" t="s">
         <v>110</v>
       </c>
@@ -4290,7 +4252,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="305" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A305" s="4" t="s">
         <v>303</v>
       </c>
@@ -4298,7 +4260,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="306" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A306" s="4" t="s">
         <v>304</v>
       </c>
@@ -4306,7 +4268,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="307" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A307" s="4" t="s">
         <v>305</v>
       </c>
@@ -4314,7 +4276,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="308" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A308" s="4" t="s">
         <v>306</v>
       </c>
@@ -4322,7 +4284,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="309" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A309" s="4" t="s">
         <v>307</v>
       </c>
@@ -4330,7 +4292,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="310" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A310" s="4" t="s">
         <v>308</v>
       </c>
@@ -4338,7 +4300,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="311" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A311" s="4" t="s">
         <v>309</v>
       </c>
@@ -4346,7 +4308,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="312" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A312" s="4" t="s">
         <v>310</v>
       </c>
@@ -4354,7 +4316,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="313" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A313" s="4" t="s">
         <v>311</v>
       </c>
@@ -4362,7 +4324,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="314" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A314" s="4" t="s">
         <v>312</v>
       </c>
@@ -4370,7 +4332,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="315" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A315" s="4" t="s">
         <v>313</v>
       </c>
@@ -4378,7 +4340,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="316" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A316" s="4" t="s">
         <v>314</v>
       </c>
@@ -4386,7 +4348,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="317" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A317" s="4" t="s">
         <v>315</v>
       </c>
@@ -4394,15 +4356,18 @@
         <v>364</v>
       </c>
     </row>
-    <row r="318" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A318" s="4" t="s">
         <v>316</v>
       </c>
       <c r="B318" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="319" spans="1:2" x14ac:dyDescent="0.25">
+        <v>366</v>
+      </c>
+      <c r="C318" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="319" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A319" s="4" t="s">
         <v>317</v>
       </c>
@@ -4410,7 +4375,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="320" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A320" s="4" t="s">
         <v>318</v>
       </c>
@@ -4767,14 +4732,14 @@
     <mergeCell ref="D8:I16"/>
   </mergeCells>
   <conditionalFormatting sqref="B2:B363">
-    <cfRule type="containsText" dxfId="5" priority="1" stopIfTrue="1" operator="containsText" text="Incomplete">
+    <cfRule type="containsText" dxfId="2" priority="1" stopIfTrue="1" operator="containsText" text="Incomplete">
       <formula>NOT(ISERROR(SEARCH("Incomplete",B2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="3" stopIfTrue="1" operator="containsText" text="Partial">
+    <cfRule type="containsText" dxfId="1" priority="2" stopIfTrue="1" operator="containsText" text="Complete">
+      <formula>NOT(ISERROR(SEARCH("Complete",B2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="0" priority="3" stopIfTrue="1" operator="containsText" text="Partial">
       <formula>NOT(ISERROR(SEARCH("Partial",B2)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="2" stopIfTrue="1" operator="containsText" text="Complete">
-      <formula>NOT(ISERROR(SEARCH("Complete",B2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>